<commit_message>
[추가] Window 4종 추가
</commit_message>
<xml_diff>
--- a/Sheet/DEM_Data.xlsx
+++ b/Sheet/DEM_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BuildSpace\DesktopEquipmentMerge\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63FD8F3-3A12-49CF-BDFF-4D7CE66F5B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AB9441-25F7-487D-A4A8-98C33F65C049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34890" yWindow="3240" windowWidth="20400" windowHeight="12675" firstSheet="2" activeTab="7" xr2:uid="{285DE2B3-C00B-4EAF-B1DF-19A1C54A570F}"/>
+    <workbookView xWindow="34890" yWindow="3240" windowWidth="20400" windowHeight="12675" firstSheet="2" activeTab="8" xr2:uid="{285DE2B3-C00B-4EAF-B1DF-19A1C54A570F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref" sheetId="10" r:id="rId1"/>
@@ -21,8 +21,9 @@
     <sheet name="Trader" sheetId="6" r:id="rId6"/>
     <sheet name="Quest" sheetId="7" r:id="rId7"/>
     <sheet name="Expedition" sheetId="11" r:id="rId8"/>
-    <sheet name="RewardProb" sheetId="12" r:id="rId9"/>
-    <sheet name="Hero" sheetId="14" r:id="rId10"/>
+    <sheet name="Lv" sheetId="15" r:id="rId9"/>
+    <sheet name="RewardProb" sheetId="12" r:id="rId10"/>
+    <sheet name="Hero" sheetId="14" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="88">
   <si>
     <t>Equipment_Name_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -392,6 +393,10 @@
   </si>
   <si>
     <t>~상인 설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -937,6 +942,104 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E275678-4570-4CA2-A5D1-8566AA5F2680}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1">
+        <v>40</v>
+      </c>
+      <c r="J2" s="1">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1">
+        <v>20</v>
+      </c>
+      <c r="L2" s="1">
+        <v>30</v>
+      </c>
+      <c r="M2" s="1">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D12FA702-3FDA-4873-9476-2B23FDC79A93}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1205,7 +1308,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5F6F4D-65E2-42F1-89B1-3A28518D62CE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1881,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3D9C64-0131-485B-B804-97154A8E94F6}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2027,95 +2132,37 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E275678-4570-4CA2-A5D1-8566AA5F2680}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90F1975-8DB0-44C6-A265-CFA567B2CE61}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1">
-        <v>40</v>
-      </c>
-      <c r="F2" s="1">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1">
-        <v>30</v>
-      </c>
-      <c r="I2" s="1">
-        <v>40</v>
-      </c>
-      <c r="J2" s="1">
-        <v>10</v>
-      </c>
-      <c r="K2" s="1">
-        <v>20</v>
-      </c>
-      <c r="L2" s="1">
-        <v>30</v>
-      </c>
-      <c r="M2" s="1">
-        <v>40</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[추가] Grayscale, Building 건설
</commit_message>
<xml_diff>
--- a/Sheet/DEM_Data.xlsx
+++ b/Sheet/DEM_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BuildSpace\DesktopEquipmentMerge\Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy05\OneDrive\문서\GitHub\DesktopEquipmentMerge\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E9C04C-081A-42C8-B6D5-9529B1A37A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EDF76C-C85C-42B3-B7AB-E471FE103035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{285DE2B3-C00B-4EAF-B1DF-19A1C54A570F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{285DE2B3-C00B-4EAF-B1DF-19A1C54A570F}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="10" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="260">
   <si>
     <t>Equipment_Name_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -918,6 +918,22 @@
   </si>
   <si>
     <t>Equipment_Res_78</t>
+  </si>
+  <si>
+    <t>원정 조건 타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원정 조건 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레벨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1393,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5073855D-C842-4656-A833-2B6B73AA17C6}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1405,9 +1421,10 @@
     <col min="2" max="2" width="19.125" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="15.375" customWidth="1"/>
+    <col min="7" max="8" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1420,8 +1437,14 @@
       <c r="E1" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G1" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>-1</v>
       </c>
@@ -1434,8 +1457,14 @@
       <c r="E2" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1448,8 +1477,14 @@
       <c r="E3" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1462,8 +1497,14 @@
       <c r="E4" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1472,6 +1513,50 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1631,7 +1716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{375FEDA8-0451-4789-BF9C-DBB1721B45C7}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1784,7 +1869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BEAE22-5922-41C3-8363-1D72AEC2DD20}">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
@@ -5929,7 +6014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF15104-731A-4C98-BA74-8497E4F21D42}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6159,10 +6244,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3D9C64-0131-485B-B804-97154A8E94F6}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6307,9 +6392,73 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>VLOOKUP(B3,TextTag!$A:$B,2,0)</f>
+        <v>던전1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f>VLOOKUP(H3,Reference!$A:$B,2,0)</f>
+        <v>아이템 개수</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f>VLOOKUP(L3,Reference!$A:$B,2,0)</f>
+        <v>없음</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q3" s="1" t="str">
+        <f>VLOOKUP(P3,Reference!$A:$B,2,0)</f>
+        <v>없음</v>
+      </c>
+      <c r="R3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>